<commit_message>
Fix display bug adjust excel style
</commit_message>
<xml_diff>
--- a/report_template/districtReport.xlsx
+++ b/report_template/districtReport.xlsx
@@ -46,8 +46,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -121,7 +122,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -138,6 +139,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -423,7 +433,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -431,7 +441,7 @@
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="53.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="6" customWidth="1"/>
     <col min="5" max="16384" width="14.625" style="1"/>
   </cols>
   <sheetData>
@@ -456,7 +466,7 @@
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
     </row>
@@ -464,7 +474,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>